<commit_message>
schematics > dcdc, switch and battery / pcb > round courner
</commit_message>
<xml_diff>
--- a/documentation/BOM.xlsx
+++ b/documentation/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t xml:space="preserve">link</t>
   </si>
@@ -70,6 +70,15 @@
     <t xml:space="preserve">MCP73831 LiPo charger</t>
   </si>
   <si>
+    <t xml:space="preserve">http://www.mouser.ch/ProductDetail/Maxim-Integrated/MAX1595EUA33+/?qs=sGAEpiMZZMtitjHzVIkrqUmW7fHvDhXHgnQoEKfsHaU%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX1595EUA33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buck/boost 3.3v dcdc</t>
+  </si>
+  <si>
     <t xml:space="preserve">conn USB Micro B femal</t>
   </si>
   <si>
@@ -91,10 +100,34 @@
     <t xml:space="preserve">push button</t>
   </si>
   <si>
+    <t xml:space="preserve">http://www.mouser.ch/ProductDetail/CK-Components/SK-12C0405-SG-15-RT/?qs=sGAEpiMZZMtHXLepoqNyVaknRufv4Zo6J8yLuspm3Zw%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK-12C0405-SG 1.5 RT</t>
+  </si>
+  <si>
     <t xml:space="preserve">switch on-off</t>
   </si>
   <si>
+    <t xml:space="preserve">http://www.mouser.ch/ProductDetail/CK-Components/KMR631NG-ULC-LFS/?qs=sGAEpiMZZMsgGjVA3toVBJ1OkFFtNMGB4KijNZUSro0%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KMR631NG ULC LFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reset push buton</t>
+  </si>
+  <si>
     <t xml:space="preserve">led RGB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.mouser.ch/ProductDetail/Linx-Technologies/BAT-HLD-002-SMT/?qs=%2fha2pyFaduilhNkyJFgy2WekJWQQ7JGY1Lox0Z3adM0%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAT-HLD-002-SMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">support CR2016</t>
   </si>
   <si>
     <t xml:space="preserve">alibaba</t>
@@ -229,19 +262,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:H15"/>
+  <dimension ref="B3:H18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.4851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9925925925926"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.1185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -288,7 +321,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>6</v>
       </c>
@@ -306,6 +339,10 @@
       </c>
       <c r="G5" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">F5*G5</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -332,46 +369,46 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="C7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>17</v>
+      </c>
       <c r="E7" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>0.7</v>
+        <v>3.88</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H7" s="0" t="n">
         <f aca="false">F7*G7</f>
-        <v>0.7</v>
+        <v>3.88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="E8" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>3.9</v>
+        <v>0.7</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H8" s="0" t="n">
         <f aca="false">F8*G8</f>
-        <v>3.9</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,102 +425,111 @@
         <v>22</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0.8</v>
+        <v>3.9</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">F9*G9</f>
-        <v>4.8</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="C10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>24</v>
+      </c>
       <c r="E10" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>0.8</v>
+        <v>0.16</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H10" s="0" t="n">
         <f aca="false">F10*G10</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="C11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="E11" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>2.5</v>
+        <v>0.97</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H11" s="0" t="n">
         <f aca="false">F11*G11</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>5</v>
+        <v>0.27</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H12" s="0" t="n">
         <f aca="false">F12*G12</f>
-        <v>5</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>32</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>3.61</v>
+        <v>2.5</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H13" s="0" t="n">
         <f aca="false">F13*G13</f>
-        <v>3.61</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="0" t="s">
@@ -493,25 +539,98 @@
         <v>35</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>2</v>
+        <v>0.28</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H14" s="0" t="n">
         <f aca="false">F14*G14</f>
+        <v>0.28</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">F15*G15</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <f aca="false">F16*G16</f>
+        <v>3.61</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="0" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H15" s="0" t="n">
-        <f aca="false">SUM(H4:H14)</f>
-        <v>30.24</v>
+      <c r="G17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <f aca="false">F17*G17</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H18" s="0" t="n">
+        <f aca="false">SUM(H4:H17)</f>
+        <v>31.5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" display="http://www.mouser.ch/Search/ProductDetail.aspx?qs=8%2f1pEl6ptNseo9Gxrhu%2fPA%3d%3d"/>
+    <hyperlink ref="C7" r:id="rId2" display="http://www.mouser.ch/ProductDetail/Maxim-Integrated/MAX1595EUA33+/?qs=sGAEpiMZZMtitjHzVIkrqUmW7fHvDhXHgnQoEKfsHaU%3d"/>
+    <hyperlink ref="C11" r:id="rId3" display="http://www.mouser.ch/ProductDetail/CK-Components/SK-12C0405-SG-15-RT/?qs=sGAEpiMZZMtHXLepoqNyVaknRufv4Zo6J8yLuspm3Zw%3d"/>
+    <hyperlink ref="C12" r:id="rId4" display="http://www.mouser.ch/ProductDetail/CK-Components/KMR631NG-ULC-LFS/?qs=sGAEpiMZZMsgGjVA3toVBJ1OkFFtNMGB4KijNZUSro0%3d"/>
+    <hyperlink ref="C14" r:id="rId5" display="http://www.mouser.ch/ProductDetail/Linx-Technologies/BAT-HLD-002-SMT/?qs=%2fha2pyFaduilhNkyJFgy2WekJWQQ7JGY1Lox0Z3adM0%3d"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
schematics > rgb led / pcb > via size route
</commit_message>
<xml_diff>
--- a/documentation/BOM.xlsx
+++ b/documentation/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
@@ -82,10 +82,10 @@
     <t xml:space="preserve">conn USB Micro B femal</t>
   </si>
   <si>
-    <t xml:space="preserve">http://www.mouser.ch/ProductDetail/PUI-Audio/SMT-1141-T-3-R/?qs=%2fha2pyFaduiCLgby5iJPqp2iGH%252b6CT48ZBFKPYK%2fGYsaasTvnsIatg%3d%3d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMT-1141-T-3-R</t>
+    <t xml:space="preserve">http://www.mouser.ch/ProductDetail/Mallory-Sonalert/AST1109MLTRQ/?qs=sGAEpiMZZMtWZVZ%2fjgUYS%252bu1KhIEHEMRsnSRypyJqVQ%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AST1109MLTRQ</t>
   </si>
   <si>
     <t xml:space="preserve">piezzo </t>
@@ -264,17 +264,15 @@
   </sheetPr>
   <dimension ref="B3:H18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.0407407407407"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -411,7 +409,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>6</v>
       </c>
@@ -425,14 +423,14 @@
         <v>22</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>3.9</v>
+        <v>3.12</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">F9*G9</f>
-        <v>3.9</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -621,16 +619,17 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H18" s="0" t="n">
         <f aca="false">SUM(H4:H17)</f>
-        <v>31.5</v>
+        <v>30.72</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" display="http://www.mouser.ch/Search/ProductDetail.aspx?qs=8%2f1pEl6ptNseo9Gxrhu%2fPA%3d%3d"/>
     <hyperlink ref="C7" r:id="rId2" display="http://www.mouser.ch/ProductDetail/Maxim-Integrated/MAX1595EUA33+/?qs=sGAEpiMZZMtitjHzVIkrqUmW7fHvDhXHgnQoEKfsHaU%3d"/>
-    <hyperlink ref="C11" r:id="rId3" display="http://www.mouser.ch/ProductDetail/CK-Components/SK-12C0405-SG-15-RT/?qs=sGAEpiMZZMtHXLepoqNyVaknRufv4Zo6J8yLuspm3Zw%3d"/>
-    <hyperlink ref="C12" r:id="rId4" display="http://www.mouser.ch/ProductDetail/CK-Components/KMR631NG-ULC-LFS/?qs=sGAEpiMZZMsgGjVA3toVBJ1OkFFtNMGB4KijNZUSro0%3d"/>
-    <hyperlink ref="C14" r:id="rId5" display="http://www.mouser.ch/ProductDetail/Linx-Technologies/BAT-HLD-002-SMT/?qs=%2fha2pyFaduilhNkyJFgy2WekJWQQ7JGY1Lox0Z3adM0%3d"/>
+    <hyperlink ref="C9" r:id="rId3" display="http://www.mouser.ch/ProductDetail/Mallory-Sonalert/AST1109MLTRQ/?qs=sGAEpiMZZMtWZVZ%2fjgUYS%252bu1KhIEHEMRsnSRypyJqVQ%3d"/>
+    <hyperlink ref="C11" r:id="rId4" display="http://www.mouser.ch/ProductDetail/CK-Components/SK-12C0405-SG-15-RT/?qs=sGAEpiMZZMtHXLepoqNyVaknRufv4Zo6J8yLuspm3Zw%3d"/>
+    <hyperlink ref="C12" r:id="rId5" display="http://www.mouser.ch/ProductDetail/CK-Components/KMR631NG-ULC-LFS/?qs=sGAEpiMZZMsgGjVA3toVBJ1OkFFtNMGB4KijNZUSro0%3d"/>
+    <hyperlink ref="C14" r:id="rId6" display="http://www.mouser.ch/ProductDetail/Linx-Technologies/BAT-HLD-002-SMT/?qs=%2fha2pyFaduilhNkyJFgy2WekJWQQ7JGY1Lox0Z3adM0%3d"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>